<commit_message>
Update 1. Data Validation - Exercise.xlsx
</commit_message>
<xml_diff>
--- a/1. Data Validation - Exercise.xlsx
+++ b/1. Data Validation - Exercise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27031"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27108"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alphad.sharepoint.com/sites/Clients/Shared Documents/HSBC/2023/12199 - HSBC EMEA - Excel Training Sheffield Grads 2023/Materials/Session 3- Enhancing Your Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgeMount\Documents\GitHub\hsbc-enhancing-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{B11D143A-4710-4F0E-95A5-2A84F5BCC283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{399C7DB6-2A39-4CC3-89D7-6A9502226605}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86413BE-477B-464E-A2DF-7216B270866E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="18915" windowHeight="12676" activeTab="1" xr2:uid="{5CAEE100-183E-4775-BB86-11B5C6F85569}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{5CAEE100-183E-4775-BB86-11B5C6F85569}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -598,8 +598,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="C2:G23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -883,11 +883,6 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="E5:E18" xr:uid="{FAC5A428-BC3D-45E0-B36B-F9FDF9B387E5}">
-      <formula1>Options</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -900,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F885D493-4446-4D86-BC9D-D34BD622A9CB}">
   <dimension ref="C2:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E18"/>
+    <sheetView showGridLines="0" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1227,15 +1222,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100265553BD9181624686A68F63ABB446DF" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ee33f439afe5f713e430bc419b9183ba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="26d2fa48-a9bb-4686-8122-5406e5c0c038" xmlns:ns3="059fecdb-ee26-4135-81c8-712a955c51df" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8a55f4bd9fbe5a9e1352735377af3810" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1501,6 +1487,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1515,14 +1510,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6098A10B-C8DB-4291-B0D8-A46701C73A06}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1D9AE19-950D-46A9-84FA-3898FBE950CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1542,6 +1529,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6098A10B-C8DB-4291-B0D8-A46701C73A06}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E85AD31-86A9-4769-90BF-EFB30A624535}">
   <ds:schemaRefs>

</xml_diff>